<commit_message>
Updates for Gentable and L2 URS
</commit_message>
<xml_diff>
--- a/DbLayouts/L4-批次作業/BankDeductDtl.xlsx
+++ b/DbLayouts/L4-批次作業/BankDeductDtl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -488,10 +488,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>AmlRsp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>繳息迄日</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -645,16 +641,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>NA:未產
-Y:已產
-N:已產，扣款金額為0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MediaCode</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>空白:未回 00:扣款成功 &gt;00 :扣款失敗
 失敗原因 : ref. CdCode ProcCode 處理說明
  ACH  : 002 + ReturnCode(2)
@@ -734,6 +720,20 @@
   <si>
     <t>EntryDate &gt;= ,AND EntryDate &lt;= ,AND RepayType =</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MediaCode</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>AmlRsp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA:未產
+Y:已產
+N:已產，檢核不正常(扣款金額為0，AML…)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1411,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -1548,7 +1548,7 @@
         <v>50</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>45</v>
@@ -1627,7 +1627,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1654,10 +1654,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>45</v>
@@ -1692,7 +1692,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>22</v>
@@ -1704,7 +1704,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1775,7 +1775,7 @@
         <v>103</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>28</v>
@@ -1864,7 +1864,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="48.6">
@@ -1872,10 +1872,10 @@
         <v>18</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>107</v>
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="32.4">
@@ -1904,7 +1904,7 @@
         <v>2</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2016,7 +2016,7 @@
         <v>70</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D33" s="28" t="s">
         <v>29</v>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2067,7 +2067,7 @@
         <v>8</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="50" customFormat="1">
@@ -2075,10 +2075,10 @@
         <v>28</v>
       </c>
       <c r="B36" s="45" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C36" s="46" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D36" s="47" t="s">
         <v>29</v>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="F36" s="48"/>
       <c r="G36" s="49" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="50" customFormat="1">
@@ -2096,10 +2096,10 @@
         <v>29</v>
       </c>
       <c r="B37" s="45" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C37" s="46" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D37" s="47" t="s">
         <v>29</v>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="F37" s="48"/>
       <c r="G37" s="49" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="31" customFormat="1" ht="64.8">
@@ -2117,7 +2117,7 @@
         <v>30</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>123</v>
+        <v>178</v>
       </c>
       <c r="C38" s="23" t="s">
         <v>60</v>
@@ -2130,7 +2130,7 @@
       </c>
       <c r="F38" s="29"/>
       <c r="G38" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="31" customFormat="1" ht="64.8">
@@ -2138,10 +2138,10 @@
         <v>31</v>
       </c>
       <c r="B39" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" s="23" t="s">
         <v>157</v>
-      </c>
-      <c r="C39" s="23" t="s">
-        <v>158</v>
       </c>
       <c r="D39" s="30" t="s">
         <v>59</v>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="F39" s="29"/>
       <c r="G39" s="22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="22.2" customHeight="1">
@@ -2159,13 +2159,13 @@
         <v>32</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C40" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" s="32" t="s">
         <v>125</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>126</v>
       </c>
       <c r="E40" s="29">
         <v>300</v>
@@ -2279,9 +2279,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -2349,10 +2349,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>118</v>
@@ -2363,7 +2363,7 @@
         <v>73</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2395,7 +2395,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>113</v>
@@ -2403,10 +2403,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>113</v>
@@ -2425,10 +2425,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>118</v>
@@ -2462,53 +2462,53 @@
   <sheetData>
     <row r="1" spans="2:6" s="43" customFormat="1">
       <c r="B1" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D1" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="40" t="s">
         <v>146</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -2517,18 +2517,18 @@
     </row>
     <row r="5" spans="2:6">
       <c r="C5" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="E6" s="41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
URS and Gentable updates
</commit_message>
<xml_diff>
--- a/DbLayouts/L4-批次作業/BankDeductDtl.xlsx
+++ b/DbLayouts/L4-批次作業/BankDeductDtl.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\SKL\DB\GenTables\L4-批次作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L4-批次作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20916" windowHeight="8472"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="180">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -298,10 +298,6 @@
   </si>
   <si>
     <t>RepayType</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>撥款</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -436,10 +432,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>BormNo</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>EntryDate DESC</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -462,10 +454,6 @@
   <si>
     <t>CustNo ASC, FacmNo ASC, PayIntDate ASC, RepayType DESC</t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>EntryDate,CustNo,FacmNo,BormNo,RepayType,PayIntDate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">EntryDate &gt;= ,AND EntryDate &lt;= , AND MediaKind = </t>
@@ -671,10 +659,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>CustNo = ,AND FacmNo = ,AND BormNo = ,AND PrevIntDate =</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>EntryDate &gt;= ,AND EntryDate &lt;= ,AND RepayType =</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -732,16 +716,24 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">CustNo = ,AND FacmNo = ,AND BormNo = ,AND RepayType = </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>findL4450EntryDateFirst</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>findL4450PrevIntDateFirst</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CustNo = ,AND FacmNo = ,AND RepayType = </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CustNo = ,AND FacmNo = ,AND PrevIntDate =</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>EntryDate,CustNo,FacmNo,RepayType,PayIntDate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1417,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -1440,7 +1432,7 @@
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>38</v>
@@ -1468,7 +1460,7 @@
       </c>
       <c r="B3" s="54"/>
       <c r="C3" s="12" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>18</v>
@@ -1507,7 +1499,7 @@
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="10"/>
@@ -1556,7 +1548,7 @@
         <v>50</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>45</v>
@@ -1599,120 +1591,121 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="145.80000000000001">
       <c r="A12" s="26">
         <v>4</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="21">
-        <v>3</v>
-      </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-    </row>
-    <row r="13" spans="1:7" ht="145.80000000000001">
+        <v>2</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="26">
         <v>5</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>28</v>
+        <v>75</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="E13" s="21">
-        <v>2</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>127</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="22"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>6</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="21">
         <v>8</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="26">
         <v>7</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>45</v>
+        <v>63</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="E15" s="21">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="32.4">
       <c r="A16" s="26">
         <v>8</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>54</v>
+        <v>148</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E16" s="21">
         <v>3</v>
       </c>
-      <c r="F16" s="24"/>
       <c r="G16" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="32.4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="26">
         <v>9</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="21">
-        <v>3</v>
+      <c r="E17" s="36">
+        <v>14</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1720,19 +1713,20 @@
         <v>10</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="36">
-        <v>14</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="21">
+        <v>2</v>
+      </c>
+      <c r="F18" s="24"/>
       <c r="G18" s="22" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1740,31 +1734,29 @@
         <v>11</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="E19" s="21">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F19" s="24"/>
-      <c r="G19" s="22" t="s">
-        <v>67</v>
-      </c>
+      <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="26">
         <v>12</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>28</v>
@@ -1775,43 +1767,45 @@
       <c r="F20" s="24"/>
       <c r="G20" s="22"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="32.4">
       <c r="A21" s="26">
         <v>13</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>28</v>
       </c>
       <c r="E21" s="21">
         <v>14</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="22"/>
-    </row>
-    <row r="22" spans="1:7" ht="32.4">
+      <c r="G21" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="26">
         <v>14</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>28</v>
+        <v>76</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="E22" s="21">
-        <v>14</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F22" s="24"/>
       <c r="G22" s="22" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1819,40 +1813,39 @@
         <v>15</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="21">
         <v>8</v>
       </c>
-      <c r="F23" s="24"/>
       <c r="G23" s="22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="48.6">
       <c r="A24" s="26">
         <v>16</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>45</v>
+        <v>94</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>29</v>
       </c>
       <c r="E24" s="21">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="48.6">
@@ -1860,59 +1853,59 @@
         <v>17</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>96</v>
+        <v>163</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="E25" s="21">
         <v>1</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="48.6">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="32.4">
       <c r="A26" s="26">
         <v>18</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>167</v>
+        <v>19</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>148</v>
+        <v>36</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="E26" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="32.4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="26">
         <v>19</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E27" s="21">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1920,16 +1913,16 @@
         <v>20</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="21">
-        <v>100</v>
+        <v>29</v>
+      </c>
+      <c r="E28" s="19">
+        <v>10</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>52</v>
@@ -1939,143 +1932,144 @@
       <c r="A29" s="26">
         <v>21</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>48</v>
+      <c r="B29" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>112</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="19">
-        <v>10</v>
-      </c>
-      <c r="G29" s="22" t="s">
-        <v>52</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E29" s="26">
+        <v>8</v>
+      </c>
+      <c r="F29" s="24"/>
+      <c r="G29" s="22"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="26">
         <v>22</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="E30" s="26">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F30" s="24"/>
-      <c r="G30" s="22"/>
+      <c r="G30" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="26">
         <v>23</v>
       </c>
-      <c r="B31" s="37" t="s">
-        <v>113</v>
+      <c r="B31" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="26">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="28">
+        <v>8</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="22" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="48.6">
       <c r="A32" s="26">
         <v>24</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>56</v>
+        <v>122</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="E32" s="28">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="48.6">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="26">
         <v>25</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" s="28" t="s">
-        <v>29</v>
+        <v>57</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="E33" s="28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="22" t="s">
-        <v>152</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="26">
         <v>26</v>
       </c>
-      <c r="B34" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="28">
+      <c r="B34" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="21">
+        <v>8</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="50" customFormat="1">
+      <c r="A35" s="44">
+        <v>27</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="44">
         <v>6</v>
       </c>
-      <c r="F34" s="24"/>
-      <c r="G34" s="22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="26">
-        <v>27</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E35" s="21">
-        <v>8</v>
-      </c>
-      <c r="G35" s="22" t="s">
-        <v>161</v>
+      <c r="F35" s="48"/>
+      <c r="G35" s="49" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="50" customFormat="1">
@@ -2083,41 +2077,41 @@
         <v>28</v>
       </c>
       <c r="B36" s="45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C36" s="46" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D36" s="47" t="s">
         <v>29</v>
       </c>
       <c r="E36" s="44">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F36" s="48"/>
       <c r="G36" s="49" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="50" customFormat="1">
-      <c r="A37" s="44">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="31" customFormat="1" ht="64.8">
+      <c r="A37" s="26">
         <v>29</v>
       </c>
-      <c r="B37" s="45" t="s">
-        <v>160</v>
-      </c>
-      <c r="C37" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="D37" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37" s="44">
-        <v>8</v>
-      </c>
-      <c r="F37" s="48"/>
-      <c r="G37" s="49" t="s">
-        <v>163</v>
+      <c r="B37" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="29">
+        <v>1</v>
+      </c>
+      <c r="F37" s="29"/>
+      <c r="G37" s="22" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="31" customFormat="1" ht="64.8">
@@ -2125,146 +2119,125 @@
         <v>30</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>60</v>
+        <v>147</v>
       </c>
       <c r="D38" s="30" t="s">
         <v>59</v>
       </c>
       <c r="E38" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F38" s="29"/>
       <c r="G38" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="31" customFormat="1" ht="64.8">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="22.2" customHeight="1">
       <c r="A39" s="26">
         <v>31</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="D39" s="30" t="s">
-        <v>59</v>
+        <v>119</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>120</v>
       </c>
       <c r="E39" s="29">
-        <v>2</v>
+        <v>300</v>
       </c>
       <c r="F39" s="29"/>
-      <c r="G39" s="22" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="22.2" customHeight="1">
+      <c r="G39" s="38"/>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="26">
         <v>32</v>
       </c>
-      <c r="B40" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="E40" s="29">
-        <v>300</v>
-      </c>
-      <c r="F40" s="29"/>
-      <c r="G40" s="38"/>
+      <c r="B40" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="21"/>
+      <c r="F40" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G40" s="35" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="26">
         <v>33</v>
       </c>
       <c r="B41" s="33" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D41" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="21">
+        <v>6</v>
+      </c>
+      <c r="F41" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="G41" s="35" t="s">
-        <v>82</v>
-      </c>
+      <c r="G41" s="35"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="26">
         <v>34</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D42" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" s="21">
-        <v>6</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E42" s="21"/>
       <c r="F42" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G42" s="35"/>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="26">
         <v>35</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D43" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="21">
+        <v>6</v>
+      </c>
+      <c r="F43" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="E43" s="21"/>
-      <c r="F43" s="24" t="s">
-        <v>81</v>
-      </c>
       <c r="G43" s="35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="26">
-        <v>36</v>
-      </c>
-      <c r="B44" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="34" t="s">
         <v>89</v>
-      </c>
-      <c r="D44" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="E44" s="21">
-        <v>6</v>
-      </c>
-      <c r="F44" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="G44" s="35" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2289,7 +2262,7 @@
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -2341,29 +2314,29 @@
         <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2371,75 +2344,75 @@
         <v>73</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2453,7 +2426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2470,80 +2443,80 @@
   <sheetData>
     <row r="1" spans="2:6" s="43" customFormat="1">
       <c r="B1" s="39" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C1" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>137</v>
-      </c>
       <c r="F1" s="40" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="42" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C2" s="42"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="42" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D3" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="41" t="s">
-        <v>145</v>
-      </c>
       <c r="F3" s="41" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="C4" s="41" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="E5" s="41" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="C7" s="41" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="C8" s="41" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>